<commit_message>
completing the wonderful binary search from interviewCamp
</commit_message>
<xml_diff>
--- a/Ques to look again.xlsx
+++ b/Ques to look again.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shriraj/Documents/InterviewCamp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D082A455-BCEF-8649-B14E-BEAA4E52DD2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFA6C227-3B0C-0A46-A9B9-96F73FAE0112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16180" xr2:uid="{3C7F39E9-9A06-6247-9FD2-599CD1CA9D43}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t xml:space="preserve">to take a loook of questions - </t>
   </si>
@@ -61,16 +61,38 @@
   </si>
   <si>
     <t>Given an array of integers, find the shortest sub array, that if sorted, results in theentire array being sorted.For example:[1,2,4,5,3,5,6,7] --&gt; [4,5,3] - If you sort from indices 2 to 4, the entire array is sorted.[1,3,5,2,6,4,7,8,9] --&gt; [3,5,2,6,4] -  If you sort from indices 1 to 5, the entire array is sorted.</t>
+  </si>
+  <si>
+    <t>Binary Search</t>
+  </si>
+  <si>
+    <t>Special Ques</t>
+  </si>
+  <si>
+    <t>Given a sorted array A that has been rotated in a cycle, find the smallest element of the array in O(log(n)) time. For example,
+[1,2,4,5,7,8] rotated by 3 gives us A = [5,7,8,1,2,4] and the smallest number is 1.
+[1,2,4,5,7,8] rotated by 1 gives us A = [8,1,2,4,5,7] and the smallest number is 1.</t>
+  </si>
+  <si>
+    <t>https://interviewcamp.io/courses/101687/lectures/2636568</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -93,13 +115,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -412,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{300D7F64-E159-CE4A-9C75-3B3DA308AF30}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -459,7 +487,27 @@
         <v>7</v>
       </c>
     </row>
+    <row r="5" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E5" r:id="rId1" xr:uid="{3513EE25-19F1-E040-B9E6-7942080E60B0}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
arrays and strings 2
</commit_message>
<xml_diff>
--- a/Ques to look again.xlsx
+++ b/Ques to look again.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shriraj/Documents/InterviewCamp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15C8D868-3F9F-8240-BE4F-A47AA9B0A63E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5881534-C858-E040-B494-27E483393530}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16180" xr2:uid="{3C7F39E9-9A06-6247-9FD2-599CD1CA9D43}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16180" activeTab="1" xr2:uid="{3C7F39E9-9A06-6247-9FD2-599CD1CA9D43}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1 (2)" sheetId="3" r:id="rId2"/>
+    <sheet name="Strings" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="23">
   <si>
     <t xml:space="preserve">to take a loook of questions - </t>
   </si>
@@ -93,6 +95,18 @@
   </si>
   <si>
     <t>Implementation of a BST</t>
+  </si>
+  <si>
+    <t>Strings</t>
+  </si>
+  <si>
+    <t>Longest Palindromic Substring</t>
+  </si>
+  <si>
+    <t>Doubt</t>
+  </si>
+  <si>
+    <t>Do it by DP way or by interview camp method</t>
   </si>
 </sst>
 </file>
@@ -460,8 +474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{300D7F64-E159-CE4A-9C75-3B3DA308AF30}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -570,4 +584,134 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10189BF8-729F-024A-95E4-F1EFB9B3E160}">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="35.33203125" customWidth="1"/>
+    <col min="4" max="4" width="75.1640625" customWidth="1"/>
+    <col min="5" max="5" width="52" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E5" r:id="rId1" xr:uid="{B1FF9BE6-1E94-DD40-AC79-16215EB73629}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{757C242C-68ED-454D-BC3B-3F7E58CA6D75}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added graph questions and some changes
</commit_message>
<xml_diff>
--- a/Ques to look again.xlsx
+++ b/Ques to look again.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shriraj/Documents/InterviewCamp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40ED6ECE-5F10-0449-9723-14E269AEC8BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDA733AE-C48E-3540-8A31-B6CAA1C9A6E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15880" xr2:uid="{3C7F39E9-9A06-6247-9FD2-599CD1CA9D43}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15820" xr2:uid="{3C7F39E9-9A06-6247-9FD2-599CD1CA9D43}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="37">
   <si>
     <t xml:space="preserve">to take a loook of questions - </t>
   </si>
@@ -148,6 +148,9 @@
   </si>
   <si>
     <t>Tre</t>
+  </si>
+  <si>
+    <t>Dutch National flag problem</t>
   </si>
 </sst>
 </file>
@@ -171,12 +174,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -192,12 +201,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -516,7 +529,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -581,6 +594,14 @@
         <v>29</v>
       </c>
     </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>36</v>
+      </c>
+    </row>
     <row r="6" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
@@ -641,13 +662,14 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
+      <c r="B14" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E14" t="s">
+      <c r="D14" s="3"/>
+      <c r="E14" s="3" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>